<commit_message>
SAFreader en ASTA index update voor levels
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/ASTA Index Current.xlsx
+++ b/src/sastadev/data/methods/ASTA Index Current.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\src\sastadev\data\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967E3B09-87E7-4BB2-8406-4578A360800A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B4BA0C-0741-4F87-84CF-0488C4B1CDD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -605,10 +605,10 @@
     <t>DELVW</t>
   </si>
   <si>
-    <t>deletie van een voegwoord</t>
-  </si>
-  <si>
     <t>onver</t>
+  </si>
+  <si>
+    <t>deletie van een vraagwoord</t>
   </si>
 </sst>
 </file>
@@ -991,10 +991,10 @@
   <dimension ref="A1:S49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
+      <selection pane="bottomRight" activeCell="Q50" sqref="Q50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1950,7 +1950,7 @@
         <v>95</v>
       </c>
       <c r="F36" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H36" t="s">
         <v>15</v>
@@ -2279,7 +2279,7 @@
         <v>130</v>
       </c>
       <c r="Q49" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
astalevels, added updated ASTA method definition
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/ASTA Index Current.xlsx
+++ b/src/sastadev/data/methods/ASTA Index Current.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\src\sastadev\data\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B4BA0C-0741-4F87-84CF-0488C4B1CDD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974E7681-6225-4389-8E30-207BA5E60F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -991,7 +991,7 @@
   <dimension ref="A1:S49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="Q50" sqref="Q50"/>

</xml_diff>

<commit_message>
reskey updates  especially for forms
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/ASTA Index Current.xlsx
+++ b/src/sastadev/data/methods/ASTA Index Current.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\methods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\src\sastadev\data\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5702438-4BE8-4DA4-9AA5-AD3B855DDEE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D46614D-9A7B-4432-8A3D-1896BF4125CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="0" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$W$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$W$49</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="199">
   <si>
     <t>ID</t>
   </si>
@@ -284,9 +284,6 @@
     <t>A032</t>
   </si>
   <si>
-    <t>A033</t>
-  </si>
-  <si>
     <t>A034</t>
   </si>
   <si>
@@ -305,9 +302,6 @@
     <t>A039</t>
   </si>
   <si>
-    <t>QA</t>
-  </si>
-  <si>
     <t>SUBVZ</t>
   </si>
   <si>
@@ -317,9 +311,6 @@
     <t>SUBPV</t>
   </si>
   <si>
-    <t>DELPV</t>
-  </si>
-  <si>
     <t>SUBLID</t>
   </si>
   <si>
@@ -536,9 +527,6 @@
     <t>asta_lex</t>
   </si>
   <si>
-    <t xml:space="preserve"> deletie van een persoonsvorm, gebruik A009 in plaats van deze</t>
-  </si>
-  <si>
     <t>asta_delpv</t>
   </si>
   <si>
@@ -563,9 +551,6 @@
     <t>getnounlemmas</t>
   </si>
   <si>
-    <t>noun en verb lemmas split up</t>
-  </si>
-  <si>
     <t>nounlemma</t>
   </si>
   <si>
@@ -639,6 +624,15 @@
   </si>
   <si>
     <t>astalemmafunction</t>
+  </si>
+  <si>
+    <t>foutenanalyse</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> deletie van een persoonsvorm</t>
+  </si>
+  <si>
+    <t>noun en verb lemmas split up; deze moet verdwijnen</t>
   </si>
 </sst>
 </file>
@@ -1018,13 +1012,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W50"/>
+  <dimension ref="A1:W49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O51" sqref="O51"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1070,31 +1064,31 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>11</v>
@@ -1113,28 +1107,28 @@
         <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H2" t="s">
         <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="L2" t="s">
         <v>15</v>
       </c>
       <c r="N2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="R2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="U2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
@@ -1157,7 +1151,7 @@
         <v>15</v>
       </c>
       <c r="N3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
@@ -1180,13 +1174,13 @@
         <v>12</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="L4" t="s">
         <v>15</v>
       </c>
       <c r="N4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="U4" t="s">
         <v>40</v>
@@ -1200,10 +1194,10 @@
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -1215,7 +1209,7 @@
         <v>15</v>
       </c>
       <c r="N5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
@@ -1226,10 +1220,10 @@
         <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -1241,7 +1235,7 @@
         <v>15</v>
       </c>
       <c r="N6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
@@ -1249,13 +1243,13 @@
         <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>89</v>
+        <v>196</v>
       </c>
       <c r="E7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>
@@ -1264,7 +1258,7 @@
         <v>15</v>
       </c>
       <c r="N7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="U7" t="s">
         <v>70</v>
@@ -1290,7 +1284,7 @@
         <v>15</v>
       </c>
       <c r="N8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
@@ -1304,19 +1298,19 @@
         <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
       </c>
       <c r="K9" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="L9" t="s">
         <v>15</v>
       </c>
       <c r="N9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
@@ -1324,25 +1318,28 @@
         <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>89</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F10" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H10" t="s">
         <v>15</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L10" t="s">
         <v>15</v>
       </c>
       <c r="N10" t="s">
-        <v>133</v>
+        <v>130</v>
+      </c>
+      <c r="U10" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
@@ -1365,7 +1362,7 @@
         <v>15</v>
       </c>
       <c r="N11" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
@@ -1388,7 +1385,7 @@
         <v>15</v>
       </c>
       <c r="N12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
@@ -1411,7 +1408,7 @@
         <v>15</v>
       </c>
       <c r="N13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
@@ -1425,7 +1422,7 @@
         <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H14" t="s">
         <v>15</v>
@@ -1434,16 +1431,16 @@
         <v>37</v>
       </c>
       <c r="K14" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="L14" t="s">
         <v>15</v>
       </c>
       <c r="N14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="Q14" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="U14" t="s">
         <v>38</v>
@@ -1457,11 +1454,11 @@
         <v>18</v>
       </c>
       <c r="E15" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" t="s">
         <v>112</v>
       </c>
-      <c r="F15" t="s">
-        <v>115</v>
-      </c>
       <c r="H15" t="s">
         <v>15</v>
       </c>
@@ -1469,7 +1466,7 @@
         <v>15</v>
       </c>
       <c r="N15" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
@@ -1477,13 +1474,13 @@
         <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>89</v>
+        <v>196</v>
       </c>
       <c r="E16" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F16" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H16" t="s">
         <v>15</v>
@@ -1492,7 +1489,7 @@
         <v>15</v>
       </c>
       <c r="N16" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
@@ -1500,13 +1497,13 @@
         <v>55</v>
       </c>
       <c r="D17" t="s">
-        <v>89</v>
+        <v>196</v>
       </c>
       <c r="E17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F17" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H17" t="s">
         <v>15</v>
@@ -1515,7 +1512,7 @@
         <v>15</v>
       </c>
       <c r="N17" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
@@ -1523,13 +1520,13 @@
         <v>56</v>
       </c>
       <c r="D18" t="s">
-        <v>89</v>
+        <v>196</v>
       </c>
       <c r="E18" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F18" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H18" t="s">
         <v>15</v>
@@ -1538,7 +1535,7 @@
         <v>15</v>
       </c>
       <c r="N18" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="U18" t="s">
         <v>69</v>
@@ -1561,17 +1558,17 @@
         <v>9</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="M19" s="3"/>
       <c r="N19" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
@@ -1594,16 +1591,16 @@
         <v>15</v>
       </c>
       <c r="K20" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="L20" t="s">
         <v>15</v>
       </c>
       <c r="N20" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="Q20" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
@@ -1623,19 +1620,19 @@
         <v>8</v>
       </c>
       <c r="K21" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="L21" t="s">
         <v>15</v>
       </c>
       <c r="N21" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="Q21" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="U21" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
@@ -1646,10 +1643,10 @@
         <v>18</v>
       </c>
       <c r="E22" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F22" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H22" t="s">
         <v>15</v>
@@ -1658,16 +1655,16 @@
         <v>10</v>
       </c>
       <c r="K22" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="L22" t="s">
         <v>15</v>
       </c>
       <c r="N22" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="Q22" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
@@ -1693,7 +1690,7 @@
         <v>15</v>
       </c>
       <c r="N23" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.3">
@@ -1710,13 +1707,13 @@
         <v>37</v>
       </c>
       <c r="L24" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="N24" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="U24" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
@@ -1730,19 +1727,19 @@
         <v>26</v>
       </c>
       <c r="F25" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H25" t="s">
         <v>15</v>
       </c>
       <c r="K25" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="L25" t="s">
         <v>15</v>
       </c>
       <c r="N25" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.3">
@@ -1759,13 +1756,13 @@
         <v>37</v>
       </c>
       <c r="L26" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="N26" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="U26" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.3">
@@ -1788,7 +1785,7 @@
         <v>15</v>
       </c>
       <c r="N27" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.3">
@@ -1805,13 +1802,13 @@
         <v>15</v>
       </c>
       <c r="K28" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="L28" t="s">
         <v>15</v>
       </c>
       <c r="N28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.3">
@@ -1819,10 +1816,10 @@
         <v>68</v>
       </c>
       <c r="D29" t="s">
-        <v>89</v>
+        <v>18</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H29" t="s">
         <v>15</v>
@@ -1831,7 +1828,7 @@
         <v>15</v>
       </c>
       <c r="N29" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="U29" t="s">
         <v>71</v>
@@ -1842,11 +1839,11 @@
         <v>80</v>
       </c>
       <c r="D30" t="s">
+        <v>196</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>91</v>
-      </c>
       <c r="H30" t="s">
         <v>15</v>
       </c>
@@ -1854,7 +1851,7 @@
         <v>15</v>
       </c>
       <c r="N30" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="U30" t="s">
         <v>72</v>
@@ -1865,10 +1862,10 @@
         <v>81</v>
       </c>
       <c r="D31" t="s">
-        <v>89</v>
+        <v>18</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H31" t="s">
         <v>15</v>
@@ -1877,7 +1874,7 @@
         <v>15</v>
       </c>
       <c r="N31" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="U31" t="s">
         <v>73</v>
@@ -1888,23 +1885,25 @@
         <v>82</v>
       </c>
       <c r="D32" t="s">
-        <v>89</v>
+        <v>18</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
+      </c>
+      <c r="F32" t="s">
+        <v>165</v>
       </c>
       <c r="H32" t="s">
         <v>15</v>
       </c>
-      <c r="K32" s="3"/>
       <c r="L32" t="s">
-        <v>123</v>
+        <v>15</v>
       </c>
       <c r="N32" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="U32" t="s">
-        <v>166</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.3">
@@ -1912,13 +1911,13 @@
         <v>83</v>
       </c>
       <c r="D33" t="s">
-        <v>89</v>
+        <v>196</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F33" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H33" t="s">
         <v>15</v>
@@ -1927,10 +1926,10 @@
         <v>15</v>
       </c>
       <c r="N33" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="U33" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
@@ -1938,13 +1937,13 @@
         <v>84</v>
       </c>
       <c r="D34" t="s">
-        <v>89</v>
+        <v>196</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F34" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H34" t="s">
         <v>15</v>
@@ -1953,10 +1952,10 @@
         <v>15</v>
       </c>
       <c r="N34" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="U34" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.3">
@@ -1964,13 +1963,10 @@
         <v>85</v>
       </c>
       <c r="D35" t="s">
-        <v>89</v>
+        <v>196</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F35" t="s">
-        <v>172</v>
+        <v>94</v>
       </c>
       <c r="H35" t="s">
         <v>15</v>
@@ -1979,10 +1975,10 @@
         <v>15</v>
       </c>
       <c r="N35" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="U35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
@@ -1990,10 +1986,10 @@
         <v>86</v>
       </c>
       <c r="D36" t="s">
-        <v>89</v>
+        <v>196</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H36" t="s">
         <v>15</v>
@@ -2002,10 +1998,10 @@
         <v>15</v>
       </c>
       <c r="N36" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="U36" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.3">
@@ -2013,10 +2009,10 @@
         <v>87</v>
       </c>
       <c r="D37" t="s">
-        <v>89</v>
+        <v>196</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H37" t="s">
         <v>15</v>
@@ -2025,131 +2021,134 @@
         <v>15</v>
       </c>
       <c r="N37" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="U37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="D38" t="s">
-        <v>89</v>
+        <v>196</v>
       </c>
       <c r="E38" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F38" t="s">
+        <v>167</v>
+      </c>
+      <c r="H38" t="s">
+        <v>15</v>
+      </c>
+      <c r="L38" t="s">
+        <v>15</v>
+      </c>
+      <c r="N38" t="s">
+        <v>130</v>
+      </c>
+      <c r="U38" t="s">
         <v>99</v>
-      </c>
-      <c r="H38" t="s">
-        <v>15</v>
-      </c>
-      <c r="L38" t="s">
-        <v>15</v>
-      </c>
-      <c r="N38" t="s">
-        <v>133</v>
-      </c>
-      <c r="U38" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D39" t="s">
-        <v>89</v>
+        <v>18</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="F39" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="H39" t="s">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="L39" t="s">
         <v>15</v>
       </c>
       <c r="N39" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="U39" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D40" t="s">
-        <v>89</v>
+        <v>196</v>
       </c>
       <c r="E40" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H40" t="s">
+        <v>120</v>
+      </c>
+      <c r="L40" t="s">
+        <v>15</v>
+      </c>
+      <c r="N40" t="s">
+        <v>130</v>
+      </c>
+      <c r="U40" t="s">
         <v>122</v>
-      </c>
-      <c r="F40" t="s">
-        <v>146</v>
-      </c>
-      <c r="H40" t="s">
-        <v>123</v>
-      </c>
-      <c r="L40" t="s">
-        <v>15</v>
-      </c>
-      <c r="N40" t="s">
-        <v>133</v>
-      </c>
-      <c r="U40" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="D41" t="s">
-        <v>89</v>
+        <v>18</v>
       </c>
       <c r="E41" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="H41" t="s">
+        <v>120</v>
+      </c>
+      <c r="L41" t="s">
+        <v>15</v>
+      </c>
+      <c r="N41" t="s">
+        <v>130</v>
+      </c>
+      <c r="U41" t="s">
         <v>126</v>
-      </c>
-      <c r="H41" t="s">
-        <v>123</v>
-      </c>
-      <c r="L41" t="s">
-        <v>15</v>
-      </c>
-      <c r="N41" t="s">
-        <v>133</v>
-      </c>
-      <c r="U41" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>128</v>
+      </c>
+      <c r="D42" t="s">
+        <v>196</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D42" t="s">
-        <v>89</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>128</v>
+      <c r="F42" t="s">
+        <v>144</v>
       </c>
       <c r="H42" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L42" t="s">
         <v>15</v>
       </c>
       <c r="N42" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="U42" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.3">
@@ -2157,48 +2156,48 @@
         <v>131</v>
       </c>
       <c r="D43" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="F43" t="s">
-        <v>147</v>
+        <v>28</v>
       </c>
       <c r="H43" t="s">
-        <v>123</v>
+        <v>15</v>
+      </c>
+      <c r="K43" t="s">
+        <v>134</v>
       </c>
       <c r="L43" t="s">
         <v>15</v>
       </c>
       <c r="N43" t="s">
-        <v>133</v>
-      </c>
-      <c r="U43" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="D44" t="s">
-        <v>16</v>
+        <v>171</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>28</v>
+        <v>171</v>
       </c>
       <c r="H44" t="s">
         <v>15</v>
       </c>
       <c r="K44" t="s">
-        <v>137</v>
+        <v>170</v>
       </c>
       <c r="L44" t="s">
         <v>15</v>
       </c>
       <c r="N44" t="s">
-        <v>157</v>
+        <v>149</v>
+      </c>
+      <c r="U44" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.3">
@@ -2206,162 +2205,136 @@
         <v>150</v>
       </c>
       <c r="D45" t="s">
-        <v>176</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="H45" t="s">
         <v>15</v>
       </c>
       <c r="K45" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="L45" t="s">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="N45" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="U45" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D46" t="s">
-        <v>154</v>
+        <v>18</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="H46" t="s">
-        <v>15</v>
-      </c>
-      <c r="K46" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="L46" t="s">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="N46" t="s">
+        <v>130</v>
+      </c>
+      <c r="R46" t="s">
+        <v>189</v>
+      </c>
+      <c r="U46" t="s">
         <v>158</v>
-      </c>
-      <c r="U46" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="D47" t="s">
-        <v>18</v>
+        <v>172</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="H47" t="s">
-        <v>123</v>
+        <v>15</v>
+      </c>
+      <c r="K47" t="s">
+        <v>173</v>
       </c>
       <c r="L47" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="N47" t="s">
-        <v>133</v>
-      </c>
-      <c r="R47" t="s">
-        <v>194</v>
+        <v>149</v>
       </c>
       <c r="U47" t="s">
-        <v>161</v>
+        <v>198</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F48" t="s">
         <v>177</v>
       </c>
-      <c r="E48" s="4" t="s">
-        <v>177</v>
-      </c>
       <c r="H48" t="s">
-        <v>15</v>
-      </c>
-      <c r="K48" t="s">
-        <v>178</v>
+        <v>120</v>
       </c>
       <c r="L48" t="s">
         <v>15</v>
       </c>
       <c r="N48" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="U48" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="D49" t="s">
-        <v>89</v>
+        <v>194</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="F49" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="H49" t="s">
-        <v>123</v>
+        <v>15</v>
+      </c>
+      <c r="K49" t="s">
+        <v>193</v>
       </c>
       <c r="L49" t="s">
         <v>15</v>
       </c>
       <c r="N49" t="s">
-        <v>133</v>
+        <v>130</v>
+      </c>
+      <c r="O49" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>192</v>
       </c>
       <c r="U49" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>195</v>
-      </c>
-      <c r="D50" t="s">
-        <v>151</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="H50" t="s">
-        <v>15</v>
-      </c>
-      <c r="K50" t="s">
-        <v>198</v>
-      </c>
-      <c r="L50" t="s">
-        <v>15</v>
-      </c>
-      <c r="N50" t="s">
-        <v>133</v>
-      </c>
-      <c r="O50" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q50" t="s">
-        <v>197</v>
-      </c>
-      <c r="U50" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W47" xr:uid="{356449EB-3FBE-4443-8528-03CDC854A576}"/>
+  <autoFilter ref="A1:W49" xr:uid="{356449EB-3FBE-4443-8528-03CDC854A576}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N28">
     <sortCondition ref="E2:E28"/>
   </sortState>

</xml_diff>

<commit_message>
Few additions to ASTA and SAFReader
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/ASTA Index Current.xlsx
+++ b/src/sastadev/data/methods/ASTA Index Current.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a3248526/git/sastadev_package/src/sastadev/data/methods/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C45B43C-7576-E445-AFBB-AE4261B64215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54423C87-204E-AA45-BED4-080E60844CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -716,9 +716,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -756,7 +756,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -862,7 +862,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1004,7 +1004,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1015,10 +1015,10 @@
   <dimension ref="A1:W49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
+      <selection pane="bottomRight" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2179,7 +2179,7 @@
         <v>147</v>
       </c>
       <c r="D44" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>171</v>
@@ -2254,7 +2254,7 @@
         <v>169</v>
       </c>
       <c r="D47" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>172</v>
@@ -2306,7 +2306,7 @@
         <v>190</v>
       </c>
       <c r="D49" t="s">
-        <v>194</v>
+        <v>148</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>148</v>

</xml_diff>

<commit_message>
nog een tijdelijke commit
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/ASTA Index Current.xlsx
+++ b/src/sastadev/data/methods/ASTA Index Current.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\src\sastadev\data\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D46614D-9A7B-4432-8A3D-1896BF4125CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1C8F41-9D63-4B22-BAD9-46C68C037D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1015,10 +1015,10 @@
   <dimension ref="A1:W49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2179,7 +2179,7 @@
         <v>147</v>
       </c>
       <c r="D44" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>171</v>
@@ -2254,7 +2254,7 @@
         <v>169</v>
       </c>
       <c r="D47" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>172</v>
@@ -2306,7 +2306,7 @@
         <v>190</v>
       </c>
       <c r="D49" t="s">
-        <v>194</v>
+        <v>148</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>148</v>

</xml_diff>